<commit_message>
update of poster 070225
</commit_message>
<xml_diff>
--- a/Version_on_pcloud/Data_processing_notebooks/Data_processing_KS20-527/Helper files/Helperfile_K20.xlsx
+++ b/Version_on_pcloud/Data_processing_notebooks/Data_processing_KS20-527/Helper files/Helperfile_K20.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cljd/Documents/Python_dev/PrePostCalderaKil_2025/Version_on_pcloud/Data_processing_notebooks/Data_processing_KS20-527/Helper files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96DE3759-A64F-A54F-A11B-F12E91261CD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD3C2B6F-157E-AA48-82F8-E2800A4BF320}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="37620" yWindow="7700" windowWidth="33620" windowHeight="19980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="172">
   <si>
     <t>filename</t>
   </si>
@@ -930,7 +930,7 @@
   <dimension ref="A1:R58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:R1048576"/>
+      <selection activeCell="M38" sqref="M38:M43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1325,6 +1325,9 @@
       <c r="L11" t="s">
         <v>11</v>
       </c>
+      <c r="M11" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -1363,6 +1366,9 @@
       <c r="L12" t="s">
         <v>12</v>
       </c>
+      <c r="M12" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -1401,6 +1407,9 @@
       <c r="L13" t="s">
         <v>13</v>
       </c>
+      <c r="M13" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -1439,6 +1448,9 @@
       <c r="L14" t="s">
         <v>89</v>
       </c>
+      <c r="M14" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
@@ -1477,6 +1489,9 @@
       <c r="L15" t="s">
         <v>89</v>
       </c>
+      <c r="M15" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
@@ -1515,8 +1530,11 @@
       <c r="L16" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M16" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1553,8 +1571,11 @@
       <c r="L17" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M17" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1591,8 +1612,11 @@
       <c r="L18" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M18" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1629,8 +1653,11 @@
       <c r="L19" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M19" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -1667,8 +1694,11 @@
       <c r="L20" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M20" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -1705,8 +1735,11 @@
       <c r="L21" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M21" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -1743,8 +1776,11 @@
       <c r="L22" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M22" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -1781,8 +1817,11 @@
       <c r="L23" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M23" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -1819,8 +1858,11 @@
       <c r="L24" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M24" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -1857,8 +1899,11 @@
       <c r="L25" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M25" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -1895,8 +1940,11 @@
       <c r="L26" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M26" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -1933,8 +1981,11 @@
       <c r="L27" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M27" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -1971,8 +2022,11 @@
       <c r="L28" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M28" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -2009,8 +2063,11 @@
       <c r="L29" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M29" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -2047,8 +2104,11 @@
       <c r="L30" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M30" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -2085,8 +2145,11 @@
       <c r="L31" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M31" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -2123,8 +2186,11 @@
       <c r="L32" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M32" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -2161,8 +2227,11 @@
       <c r="L33" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M33" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -2199,8 +2268,11 @@
       <c r="L34" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M34" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -2237,8 +2309,11 @@
       <c r="L35" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M35" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -2275,8 +2350,11 @@
       <c r="L36" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M36" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>37</v>
       </c>
@@ -2313,8 +2391,11 @@
       <c r="L37" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M37" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>38</v>
       </c>
@@ -2346,7 +2427,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>39</v>
       </c>
@@ -2378,7 +2459,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -2410,7 +2491,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>41</v>
       </c>
@@ -2442,7 +2523,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -2474,7 +2555,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>43</v>
       </c>
@@ -2506,7 +2587,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>44</v>
       </c>
@@ -2543,8 +2624,11 @@
       <c r="L44" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M44" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>45</v>
       </c>
@@ -2581,8 +2665,11 @@
       <c r="L45" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M45" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>46</v>
       </c>
@@ -2619,8 +2706,11 @@
       <c r="L46" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M46" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>47</v>
       </c>
@@ -2657,8 +2747,11 @@
       <c r="L47" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M47" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>48</v>
       </c>
@@ -2695,8 +2788,11 @@
       <c r="L48" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M48" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>49</v>
       </c>
@@ -2733,8 +2829,11 @@
       <c r="L49" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M49" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>50</v>
       </c>
@@ -2771,8 +2870,11 @@
       <c r="L50" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M50" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>51</v>
       </c>
@@ -2809,8 +2911,11 @@
       <c r="L51" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M51" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>52</v>
       </c>
@@ -2847,8 +2952,11 @@
       <c r="L52" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M52" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>53</v>
       </c>
@@ -2885,8 +2993,11 @@
       <c r="L53" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M53" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>54</v>
       </c>
@@ -2923,8 +3034,11 @@
       <c r="L54" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M54" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>55</v>
       </c>
@@ -2961,8 +3075,11 @@
       <c r="L55" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M55" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>56</v>
       </c>
@@ -2999,8 +3116,11 @@
       <c r="L56" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M56" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>57</v>
       </c>
@@ -3037,8 +3157,11 @@
       <c r="L57" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M57" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>58</v>
       </c>
@@ -3074,6 +3197,9 @@
       </c>
       <c r="L58" t="s">
         <v>58</v>
+      </c>
+      <c r="M58" t="s">
+        <v>164</v>
       </c>
     </row>
   </sheetData>

</xml_diff>